<commit_message>
maj analyse courbe model5
</commit_message>
<xml_diff>
--- a/Securite/Model5/adversarial/analyse_courbe_model5.xlsx
+++ b/Securite/Model5/adversarial/analyse_courbe_model5.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0216e4c439e2ba0d/Documents/Hugo/ISMIN/Cours/S9/E_IA/Projet/Github/ES_IA_Embedded_Project/Securite/Model5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0216e4c439e2ba0d/Documents/Hugo/ISMIN/Cours/S9/E_IA/Projet/Github/ES_IA_Embedded_Project/Securite/Model5/adversarial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{F11EAFFB-6C6F-44AE-A85F-9A7CD9901D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54CC52CE-1342-4C78-B6F4-89146938DFF1}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{F11EAFFB-6C6F-44AE-A85F-9A7CD9901D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB6800CA-A7D2-4556-8E6F-42006C212959}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E85540B8-82F7-4C5F-ACE8-F22BD23D7AEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -497,8 +494,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7438325A-D127-460F-94D1-6C40B15CF93B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{C90053DF-AF57-447C-BB00-AF4282443E3F}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -506,18 +503,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{411A02FD-E111-4BF4-89C6-EB5453A8A726}" type="YVALUE">
+                    <a:fld id="{7761C286-FC05-4717-80DB-5FB0B8B8378A}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -544,8 +541,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1426E415-7D17-474E-A5C0-85A1D4EB5A4B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{45924519-4391-4071-9475-36781BD098F8}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -553,18 +550,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{AFB26FB0-2C0D-4D98-918A-8393925A71EA}" type="YVALUE">
+                    <a:fld id="{8084A850-4D5A-4902-8A5A-6CD42F7092AE}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -591,8 +588,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71C6B462-CCD6-4E2D-B2F8-AC5085A27772}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{516125C5-5894-40C9-BD85-0BF678AE668D}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -600,18 +597,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{2F8CA4C0-F086-4F09-BD52-49CA78A74304}" type="YVALUE">
+                    <a:fld id="{4B66E3FD-B079-4ACE-BE30-E4596647DB6E}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -638,8 +635,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47ED8E01-D90B-4C7E-8CAC-264C3D6F01DD}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{57D87EE9-5109-41FC-92E8-31ACB879A835}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -647,18 +644,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{29E67E23-7EA6-46C2-933C-D08A03AB38E5}" type="YVALUE">
+                    <a:fld id="{A63B0DB6-F9F8-4939-A171-955DC280EFC4}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -685,8 +682,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EE911F2-9D5B-436F-BB2A-7669A5DA2282}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{66D201EF-E4E7-4551-B377-FD64951B268D}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -694,18 +691,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{3AA73102-ADFF-4E8A-B43F-5B2B1C1CEF5B}" type="YVALUE">
+                    <a:fld id="{BDB7DCA3-ACC8-488A-971D-6663D4F0931F}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -732,8 +729,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBD3679E-220D-4543-BFC5-17F742EAE27D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D053B1C9-7A38-4118-85CE-CB4F73F0265F}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -741,18 +738,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{47FA72B7-77C5-42F0-8AA3-EF7E10A14D7F}" type="YVALUE">
+                    <a:fld id="{5E73B6A3-9D1A-4F0B-9DB5-02C062A7E0DD}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -779,8 +776,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{560F1CED-DEAB-4D43-B492-1BEDE8DA85A9}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{4E0A25AE-9C85-444C-B273-9B26606D41FE}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -788,18 +785,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{FD180D9C-A89E-4D1D-8913-494548B2C240}" type="YVALUE">
+                    <a:fld id="{F4602744-4402-4BF4-AAFC-25E292DB7483}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -826,8 +823,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0C2CBF2-9A3D-4240-9C10-867EBB4E520D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{83CBD273-4071-445B-825B-C65D9840AEE8}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -835,18 +832,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{5EE340A7-D60F-436E-A905-92F6159C29EF}" type="YVALUE">
+                    <a:fld id="{CD1CB296-02E9-42ED-A082-F15CC41B917D}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -873,8 +870,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A219C8C7-A5C8-4418-9B08-53A9F2F5CFA7}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9EB9F8C8-E149-4602-8DD1-A8A265EEEDD0}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -882,18 +879,18 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{DA9E93BF-379A-451E-AD6D-60F6E2F18A89}" type="YVALUE">
+                    <a:fld id="{8625C92D-8078-4CE8-98A4-B02E0E66D3E3}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
-                      <a:t>[VALEUR Y]</a:t>
+                      <a:t>[VALEUR X]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
@@ -937,8 +934,8 @@
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -2020,194 +2017,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Feuil1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Accuracy</v>
-          </cell>
-          <cell r="B1"/>
-          <cell r="C1"/>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Clean</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>FGM</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>PGD (step;budget)</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>78.36</v>
-          </cell>
-          <cell r="B3">
-            <v>58.09</v>
-          </cell>
-          <cell r="C3">
-            <v>49.69</v>
-          </cell>
-          <cell r="D3">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="E3">
-            <v>5.0000000000000001E-4</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>79.95</v>
-          </cell>
-          <cell r="B4">
-            <v>44.04</v>
-          </cell>
-          <cell r="C4">
-            <v>25.88</v>
-          </cell>
-          <cell r="D4">
-            <v>0.01</v>
-          </cell>
-          <cell r="E4">
-            <v>0.01</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>78.75</v>
-          </cell>
-          <cell r="B5">
-            <v>42.69</v>
-          </cell>
-          <cell r="C5">
-            <v>28.06</v>
-          </cell>
-          <cell r="D5">
-            <v>0.01</v>
-          </cell>
-          <cell r="E5">
-            <v>1E-3</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>77.58</v>
-          </cell>
-          <cell r="B6">
-            <v>23.6</v>
-          </cell>
-          <cell r="C6">
-            <v>10.83</v>
-          </cell>
-          <cell r="D6">
-            <v>0.05</v>
-          </cell>
-          <cell r="E6">
-            <v>0.02</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>79.95</v>
-          </cell>
-          <cell r="B7">
-            <v>17.79</v>
-          </cell>
-          <cell r="C7">
-            <v>11.16</v>
-          </cell>
-          <cell r="D7">
-            <v>0.05</v>
-          </cell>
-          <cell r="E7">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>79.900000000000006</v>
-          </cell>
-          <cell r="B8">
-            <v>15.03</v>
-          </cell>
-          <cell r="C8">
-            <v>6.9</v>
-          </cell>
-          <cell r="D8">
-            <v>0.1</v>
-          </cell>
-          <cell r="E8">
-            <v>0.05</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>80.290000000000006</v>
-          </cell>
-          <cell r="B9">
-            <v>10.44</v>
-          </cell>
-          <cell r="C9">
-            <v>10.49</v>
-          </cell>
-          <cell r="D9">
-            <v>0.3</v>
-          </cell>
-          <cell r="E9">
-            <v>0.01</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>78.09</v>
-          </cell>
-          <cell r="B10">
-            <v>14.65</v>
-          </cell>
-          <cell r="C10">
-            <v>10.41</v>
-          </cell>
-          <cell r="D10">
-            <v>0.3</v>
-          </cell>
-          <cell r="E10">
-            <v>0.03</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>79.05</v>
-          </cell>
-          <cell r="B11">
-            <v>11.75</v>
-          </cell>
-          <cell r="C11">
-            <v>7.23</v>
-          </cell>
-          <cell r="D11">
-            <v>0.5</v>
-          </cell>
-          <cell r="E11">
-            <v>0.05</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -2532,7 +2341,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>